<commit_message>
Added new feature file
</commit_message>
<xml_diff>
--- a/lib/data/data.xlsx
+++ b/lib/data/data.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B25"/>
+  <dimension ref="A1:D25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -432,6 +432,16 @@
           <t>Contact</t>
         </is>
       </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Experience</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>Status</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -444,6 +454,16 @@
           <t>manju.johnson@atmecs.com</t>
         </is>
       </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>3 - 8 Years</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>Open Position</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -456,6 +476,16 @@
           <t>dinesh.avvari@atmecs.com</t>
         </is>
       </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>10 - 14 Years</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>Open Position</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -468,6 +498,16 @@
           <t>manju.johnson@atmecs.com</t>
         </is>
       </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>4 - 8 Years</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>Open Position</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -480,6 +520,16 @@
           <t>mubarak.shaik@atmecs.com</t>
         </is>
       </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>8 - 12 Years</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>Open Position</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -492,6 +542,16 @@
           <t>patitapaban.pallai@atmecs.com</t>
         </is>
       </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>4 - 8 Years</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>Open Position</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -504,6 +564,16 @@
           <t>dinesh.avvari@atmecs.com</t>
         </is>
       </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>3 - 10 Years</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>Open Position</t>
+        </is>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -516,6 +586,16 @@
           <t>anthony.chai@atmecs.com</t>
         </is>
       </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>3 - 5 Years</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>Open Position</t>
+        </is>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -528,6 +608,16 @@
           <t>patitapaban.pallai@atmecs.com</t>
         </is>
       </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>3 - 8 Years</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>Open Position</t>
+        </is>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -540,6 +630,16 @@
           <t>mubarak.shaik@atmecs.com</t>
         </is>
       </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>3 - 6 Years</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>Open Position</t>
+        </is>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -552,6 +652,16 @@
           <t>anthony.chai@atmecs.com</t>
         </is>
       </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>10 - 14 Years</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>Open Position</t>
+        </is>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -564,6 +674,16 @@
           <t>manju.johnson@atmecs.com</t>
         </is>
       </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>4 - 8 Years</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>Open Position</t>
+        </is>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -576,6 +696,16 @@
           <t>dinesh.avvari@atmecs.com</t>
         </is>
       </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>3 - 10 Years</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>Open Position</t>
+        </is>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -588,6 +718,16 @@
           <t>susheel.golla@atmecs.com</t>
         </is>
       </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>2 - 5 Years</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>Open Position</t>
+        </is>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -600,6 +740,16 @@
           <t>anthony.chai@atmecs.com</t>
         </is>
       </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>3 - 8 Years</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>Open Position</t>
+        </is>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -612,6 +762,16 @@
           <t>dinesh.avvari@atmecs.com</t>
         </is>
       </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>3 - 8 Years</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>Open Position</t>
+        </is>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -624,6 +784,16 @@
           <t>dinesh.avvari@atmecs.com</t>
         </is>
       </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>3 - 8 Years</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>Open Position</t>
+        </is>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -636,6 +806,16 @@
           <t>mubarak.shaik@atmecs.com</t>
         </is>
       </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>4 - 8 Years</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>Open Position</t>
+        </is>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -648,6 +828,16 @@
           <t>mubarak.shaik@atmecs.com</t>
         </is>
       </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>8 - 14 Years</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>Open Position</t>
+        </is>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -660,6 +850,16 @@
           <t>santhosh.rajan@atmecs.com</t>
         </is>
       </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>4 - 8 Years</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>Open Position</t>
+        </is>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -672,6 +872,16 @@
           <t>santhosh.rajan@atmecs.com</t>
         </is>
       </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>3 - 8 Years</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>Open Position</t>
+        </is>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -684,6 +894,16 @@
           <t>susheel.golla@atmecs.com</t>
         </is>
       </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>3 - 6 Years</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>Open Position</t>
+        </is>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -696,6 +916,16 @@
           <t>patitapaban.pallai@atmecs.com</t>
         </is>
       </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>3 - 6 Years</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>Open Position</t>
+        </is>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
@@ -708,6 +938,16 @@
           <t>dinesh.avvari@atmecs.com</t>
         </is>
       </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>3 - 8 Years</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>Open Position</t>
+        </is>
+      </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
@@ -718,6 +958,16 @@
       <c r="B25" t="inlineStr">
         <is>
           <t>manju.johnson@atmecs.com</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>3 - 8 Years</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>Open Position</t>
         </is>
       </c>
     </row>

</xml_diff>